<commit_message>
added account creatn details
</commit_message>
<xml_diff>
--- a/LiveProjectPractice/src/test/resources/Testdata/TestData.xlsx
+++ b/LiveProjectPractice/src/test/resources/Testdata/TestData.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\git\LiveProjectPract\LiveProjectPractice\src\test\resources\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCF3B665-9721-4278-8503-D254E9F8EC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F2989A-CC3D-40B3-8178-095DA6C7C686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B5A5013C-4ECE-48F0-8913-87ABBBC9505A}"/>
+    <workbookView xWindow="2800" yWindow="2800" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{B5A5013C-4ECE-48F0-8913-87ABBBC9505A}"/>
   </bookViews>
   <sheets>
     <sheet name="credentials" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="accountCreationdetails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Username</t>
   </si>
@@ -47,6 +47,81 @@
   </si>
   <si>
     <t>admin@123</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Namee</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City </t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>raja</t>
+  </si>
+  <si>
+    <t>BabbLe@gmail.com</t>
+  </si>
+  <si>
+    <t>mr</t>
+  </si>
+  <si>
+    <t>ran1231</t>
+  </si>
+  <si>
+    <t>kaja</t>
+  </si>
+  <si>
+    <t>hyderabad</t>
+  </si>
+  <si>
+    <t>matagat</t>
+  </si>
+  <si>
+    <t>njhggd</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>August</t>
   </si>
 </sst>
 </file>
@@ -411,7 +486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5306DA-C6E2-4B7D-909D-7A4F7AC1B931}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -448,12 +523,125 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E84826-13E8-4FE7-B2E8-15CB362432D8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:P2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="18.08984375" customWidth="1"/>
+    <col min="8" max="8" width="10.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" customWidth="1"/>
+    <col min="12" max="12" width="11.08984375" customWidth="1"/>
+    <col min="15" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2">
+        <v>2005</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2">
+        <v>637465</v>
+      </c>
+      <c r="P2">
+        <v>7344253663</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{46F3BD4C-E33C-40F3-BD8F-264DF059DFC9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>